<commit_message>
Se terminan modificaciones del modulo de compras
</commit_message>
<xml_diff>
--- a/Analisis/SPRINT/Sprint7.xlsx
+++ b/Analisis/SPRINT/Sprint7.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\comercializadora\Analisis\SPRINT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DocumentosCMV\respaldo c\proyectos\comercializadora\Analisis\SPRINT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{358B07B5-2134-4D89-9F20-DD798703F625}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{CF8223C1-468B-4922-B4D2-E853FF9B6A7E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990"/>
   </bookViews>
   <sheets>
     <sheet name="Compras" sheetId="1" r:id="rId1"/>
@@ -220,7 +219,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7">
     <font>
       <sz val="11"/>
@@ -310,11 +309,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -326,16 +322,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="5"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -347,6 +334,19 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="5"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -753,96 +753,96 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5561E258-0D5A-43AC-8196-86268693512B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="59.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.7109375" customWidth="1"/>
-    <col min="12" max="12" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="64" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.7265625" customWidth="1"/>
+    <col min="12" max="12" width="17.54296875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="26.81640625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="21" customWidth="1"/>
-    <col min="15" max="15" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="24.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:17">
-      <c r="A2" t="s">
+      <c r="A2" s="12" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="30">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:17" ht="29">
+      <c r="A3" s="15" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:17">
-      <c r="A4" t="s">
+      <c r="A4" s="12" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="30">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:17" ht="29">
+      <c r="A5" s="15" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:17">
-      <c r="A6" t="s">
+      <c r="A6" s="12" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:17">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="15" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:17">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="16" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:17">
-      <c r="K11" s="7" t="s">
+      <c r="K11" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="L11" s="7"/>
-      <c r="M11" s="7"/>
-      <c r="N11" s="7"/>
-      <c r="O11" s="7"/>
-      <c r="P11" s="7"/>
-      <c r="Q11" s="7"/>
+      <c r="L11" s="13"/>
+      <c r="M11" s="13"/>
+      <c r="N11" s="13"/>
+      <c r="O11" s="13"/>
+      <c r="P11" s="13"/>
+      <c r="Q11" s="13"/>
     </row>
     <row r="12" spans="1:17">
-      <c r="K12" s="2" t="s">
+      <c r="K12" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="L12" s="2" t="s">
+      <c r="L12" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="M12" s="2" t="s">
+      <c r="M12" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="N12" s="2" t="s">
+      <c r="N12" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="O12" s="2" t="s">
+      <c r="O12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="P12" s="2" t="s">
+      <c r="P12" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="Q12" s="2" t="s">
+      <c r="Q12" s="1" t="s">
         <v>43</v>
       </c>
     </row>
@@ -955,19 +955,19 @@
       </c>
     </row>
     <row r="26" spans="11:17">
-      <c r="K26" s="8" t="s">
+      <c r="K26" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="L26" s="8" t="s">
+      <c r="L26" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="M26" s="8" t="s">
+      <c r="M26" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="N26" s="8" t="s">
+      <c r="N26" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="O26" s="8" t="s">
+      <c r="O26" s="6" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1067,84 +1067,84 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEA772AD-CEA1-47FE-8085-296D93CC1B19}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="68.7109375" customWidth="1"/>
+    <col min="1" max="1" width="68.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:15">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="15.75">
-      <c r="A3" s="5" t="s">
+    <row r="3" spans="1:15" ht="15.5">
+      <c r="A3" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="29.25">
-      <c r="A4" s="6" t="s">
+    <row r="4" spans="1:15" ht="28.5">
+      <c r="A4" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:15">
-      <c r="K5" s="10" t="s">
+      <c r="K5" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="L5" s="10"/>
-      <c r="M5" s="10"/>
-      <c r="N5" s="10"/>
-      <c r="O5" s="10"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="14"/>
+      <c r="N5" s="14"/>
+      <c r="O5" s="14"/>
     </row>
     <row r="6" spans="1:15">
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="F6" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="11" t="s">
+      <c r="G6" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="H6" s="11" t="s">
+      <c r="H6" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="K6" s="11" t="s">
+      <c r="K6" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="L6" s="11" t="s">
+      <c r="L6" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="M6" s="11" t="s">
+      <c r="M6" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="N6" s="11" t="s">
+      <c r="N6" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="O6" s="11" t="s">
+      <c r="O6" s="7" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:15">
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="C7" s="13">
+      <c r="C7" s="9">
         <v>5.5</v>
       </c>
       <c r="F7" t="s">
@@ -1175,10 +1175,10 @@
       </c>
     </row>
     <row r="8" spans="1:15">
-      <c r="B8" s="13">
+      <c r="B8" s="9">
         <v>12</v>
       </c>
-      <c r="C8" s="13">
+      <c r="C8" s="9">
         <v>5</v>
       </c>
       <c r="F8" t="s">
@@ -1209,10 +1209,10 @@
       </c>
     </row>
     <row r="9" spans="1:15">
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="C9" s="13">
+      <c r="C9" s="9">
         <v>4.5</v>
       </c>
       <c r="F9" t="s">
@@ -1226,69 +1226,69 @@
       </c>
     </row>
     <row r="10" spans="1:15">
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="C10" s="13">
+      <c r="C10" s="9">
         <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:15">
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="C11" s="13">
+      <c r="C11" s="9">
         <v>3.5</v>
       </c>
     </row>
     <row r="14" spans="1:15">
-      <c r="B14" s="15"/>
+      <c r="B14" s="11"/>
     </row>
     <row r="15" spans="1:15">
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="C15" s="7" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:15">
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="C16" s="13">
+      <c r="C16" s="9">
         <v>6.5</v>
       </c>
     </row>
     <row r="17" spans="2:3">
-      <c r="B17" s="13">
+      <c r="B17" s="9">
         <v>12</v>
       </c>
-      <c r="C17" s="13">
+      <c r="C17" s="9">
         <v>6</v>
       </c>
     </row>
     <row r="18" spans="2:3">
-      <c r="B18" s="14" t="s">
+      <c r="B18" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="C18" s="13">
+      <c r="C18" s="9">
         <v>5.5</v>
       </c>
     </row>
     <row r="19" spans="2:3">
-      <c r="B19" s="13" t="s">
+      <c r="B19" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="C19" s="13">
+      <c r="C19" s="9">
         <v>5</v>
       </c>
     </row>
     <row r="20" spans="2:3">
-      <c r="B20" s="13" t="s">
+      <c r="B20" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="C20" s="13">
+      <c r="C20" s="9">
         <v>4.5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
observacion en el modulo de ventas
en el modulo de ventas cuando cambias  forma de pago a otra en el select se demora como 2 a 3 segundos en hacer el cambio
</commit_message>
<xml_diff>
--- a/Analisis/SPRINT/Sprint7.xlsx
+++ b/Analisis/SPRINT/Sprint7.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\comercializadora\Analisis\SPRINT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{627C5130-ED05-414A-990C-D91DDF80D250}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B25BF438-9159-4078-92B1-DDE67539CBE4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="69">
   <si>
     <t>Compras</t>
   </si>
@@ -230,6 +230,9 @@
   </si>
   <si>
     <t>{{DapperRow, Estatus = '-1', error_procedure = 'SP_INSERTA_ACTUALIZA_PRODUCTOS', error_line = '91', Mensaje = 'Cannot insert explicit value for identity column in table 'Productos' when IDENTITY_INSERT is set to OFF.'}}</t>
+  </si>
+  <si>
+    <t>en el modulo de ventas cuando cambias  forma de pago a otra en el select se demora como 2 a 3 segundos en hacer el cambio</t>
   </si>
 </sst>
 </file>
@@ -325,7 +328,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -357,6 +360,9 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="5"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -364,7 +370,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -476,15 +482,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>1</xdr:colOff>
       <xdr:row>37</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>227644</xdr:colOff>
-      <xdr:row>69</xdr:row>
-      <xdr:rowOff>18095</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>85639</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -507,8 +513,52 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7239000" y="8001000"/>
-          <a:ext cx="7647619" cy="7638095"/>
+          <a:off x="7772401" y="8001000"/>
+          <a:ext cx="4105274" cy="3895639"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>74611</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Imagen 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DECA3819-A92A-4464-8731-A4A35F0CC6AE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7772400" y="12192000"/>
+          <a:ext cx="6323011" cy="5972175"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -817,10 +867,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q40"/>
+  <dimension ref="A1:Q54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B28" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView tabSelected="1" topLeftCell="B22" workbookViewId="0">
+      <selection activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -877,15 +927,15 @@
       </c>
     </row>
     <row r="11" spans="1:17">
-      <c r="K11" s="15" t="s">
+      <c r="K11" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="L11" s="15"/>
-      <c r="M11" s="15"/>
-      <c r="N11" s="15"/>
-      <c r="O11" s="15"/>
-      <c r="P11" s="15"/>
-      <c r="Q11" s="15"/>
+      <c r="L11" s="16"/>
+      <c r="M11" s="16"/>
+      <c r="N11" s="16"/>
+      <c r="O11" s="16"/>
+      <c r="P11" s="16"/>
+      <c r="Q11" s="16"/>
     </row>
     <row r="12" spans="1:17">
       <c r="K12" s="1" t="s">
@@ -1137,7 +1187,7 @@
       <c r="B35">
         <v>2</v>
       </c>
-      <c r="C35" s="17" t="s">
+      <c r="C35" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1145,13 +1195,21 @@
       <c r="B38">
         <v>3</v>
       </c>
-      <c r="C38" s="17" t="s">
+      <c r="C38" s="15" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="40" spans="2:3" ht="120">
-      <c r="C40" s="17" t="s">
+    <row r="40" spans="2:3" ht="90">
+      <c r="C40" s="15" t="s">
         <v>67</v>
+      </c>
+    </row>
+    <row r="54" spans="2:3" ht="45">
+      <c r="B54">
+        <v>4</v>
+      </c>
+      <c r="C54" s="18" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1198,13 +1256,13 @@
       </c>
     </row>
     <row r="5" spans="1:15">
-      <c r="K5" s="16" t="s">
+      <c r="K5" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="L5" s="16"/>
-      <c r="M5" s="16"/>
-      <c r="N5" s="16"/>
-      <c r="O5" s="16"/>
+      <c r="L5" s="17"/>
+      <c r="M5" s="17"/>
+      <c r="N5" s="17"/>
+      <c r="O5" s="17"/>
     </row>
     <row r="6" spans="1:15">
       <c r="B6" s="7" t="s">

</xml_diff>